<commit_message>
DE233274: service map upload done
</commit_message>
<xml_diff>
--- a/database/files/prof/business-upload/product_classification_upload_template.xlsx
+++ b/database/files/prof/business-upload/product_classification_upload_template.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="HWSW Split%" sheetId="1" r:id="rId1"/>
+    <sheet name="HWSW Split% Upload" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="80000"/>
 </workbook>
@@ -448,35 +448,35 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -487,12 +487,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>